<commit_message>
Halfway through adding TSI inversion - Debugged and improved Twomey-Markowski
</commit_message>
<xml_diff>
--- a/inputs/dma_params_new.xlsx
+++ b/inputs/dma_params_new.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmdnkr\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFD6A81-94E7-437A-AED5-A7DCF4719748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDADBED8-DBFE-4EF1-9BFC-62B420C71BBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4065" yWindow="4065" windowWidth="21600" windowHeight="11295" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
   </bookViews>
   <sheets>
-    <sheet name="13SEP24" sheetId="7" r:id="rId1"/>
+    <sheet name="13SEP24_SWEEP_ON_FUEL" sheetId="7" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,15 +27,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
-    <t>f_add</t>
-  </si>
-  <si>
     <t>1:3</t>
   </si>
   <si>
-    <t>f_name</t>
-  </si>
-  <si>
     <t>sid</t>
   </si>
   <si>
@@ -72,7 +66,13 @@
     <t>4:7</t>
   </si>
   <si>
-    <t>D:\Hamed\CND\PhD\Experiments\PFA-RH122\PFA results\SMPS\SMPS-HN-Desktop-DEC24\Raw</t>
+    <t>D:\HN\AUG24Onward\Thesis-03Dec24\SMPS-HN-Desktop\Data\Raw</t>
+  </si>
+  <si>
+    <t>f_add_raw</t>
+  </si>
+  <si>
+    <t>f_name_raw</t>
   </si>
 </sst>
 </file>
@@ -82,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,171 +466,171 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="34" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="2" max="2" width="29.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.25" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="2"/>
+    <col min="5" max="5" width="9.125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="E2" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75">
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5">
         <v>2.5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" s="4">
         <v>20</v>
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75">
       <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E4" s="4">
         <v>20</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="5">
         <v>2.5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75">
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5">
         <v>2.5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" s="4">
         <v>20</v>
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="5">
         <v>2.5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="5">
         <v>2.5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="5">
         <v>2.5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" s="5">
         <v>2.5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="3"/>
     </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="2" customFormat="1">
       <c r="A28" s="3"/>
       <c r="C28" s="5"/>
       <c r="E28" s="4"/>
@@ -638,7 +638,7 @@
       <c r="G28"/>
       <c r="H28"/>
     </row>
-    <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" s="5" customFormat="1">
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="D48" s="2"/>

</xml_diff>

<commit_message>
Various bugs in 1d inversion procedure resolved
</commit_message>
<xml_diff>
--- a/inputs/dma_params_new.xlsx
+++ b/inputs/dma_params_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCD30A3-3BFA-4A06-B54F-E39FDCD308FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AC6D2B-CBB6-4EFE-A8C6-D4FD343EEC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
   </bookViews>
   <sheets>
     <sheet name="13SEP24_SWEEP_ON_FUEL" sheetId="7" r:id="rId1"/>
@@ -72,7 +72,7 @@
     <t>f_name_raw</t>
   </si>
   <si>
-    <t>D:\Hamed\CND\PhD\Experiments\PFA-RH122\PFA results\SMPS\SMPS-HN-Desktop-DEC24\Raw</t>
+    <t>D:\Hamed\CND\PhD\Experiments\PFA-RH122\PFA results\SMPS\SMPS-HN-Desktop-DEC24\Data\Raw</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Skewness and kurtosis added
</commit_message>
<xml_diff>
--- a/inputs/dma_params_new.xlsx
+++ b/inputs/dma_params_new.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AC6D2B-CBB6-4EFE-A8C6-D4FD343EEC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C699AFD-B7A2-42A4-8894-DEEC4C27FE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
   </bookViews>
   <sheets>
     <sheet name="13SEP24_SWEEP_ON_FUEL" sheetId="7" r:id="rId1"/>
+    <sheet name="23JUL24_SWEEP_ON_AIR" sheetId="8" r:id="rId2"/>
+    <sheet name="20JUL24_SWEEP_ON_NITROGEN" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="39">
   <si>
     <t>1:3</t>
   </si>
@@ -73,6 +75,75 @@
   </si>
   <si>
     <t>D:\Hamed\CND\PhD\Experiments\PFA-RH122\PFA results\SMPS\SMPS-HN-Desktop-DEC24\Data\Raw</t>
+  </si>
+  <si>
+    <t>2024-07-23_105221_SMPS</t>
+  </si>
+  <si>
+    <t>5:7</t>
+  </si>
+  <si>
+    <t>2024-07-23_114958_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_143207_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_180812_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_155349_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_193542_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_145054_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_183014_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_161641_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_195749_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_150820_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_185212_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_164902_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-23_201626_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-20_210133_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-20_213658_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-20_224040_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-20_222608_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-20_230642_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-20_232313_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-20_234336_SMPS</t>
+  </si>
+  <si>
+    <t>D:\Hamed\CND\PhD\Experiments\PFA-RH122\PFA results\SMPS\SMPS_laptop_datafiles_DEC24\Raw</t>
   </si>
 </sst>
 </file>
@@ -465,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E154B3E6-2BDE-4817-B65C-F71F8F992F62}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -651,4 +722,446 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E1FF8C-F2C6-4468-9BAB-5FF356FF2B49}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="5">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A154C9C-AB65-4231-8298-10E3CEF878B7}">
+  <dimension ref="A1:H47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>20</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="C27" s="5"/>
+      <c r="E27" s="4"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+    </row>
+    <row r="47" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="4"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor debugging in legend and progress toolbar
</commit_message>
<xml_diff>
--- a/inputs/dma_params_new.xlsx
+++ b/inputs/dma_params_new.xlsx
@@ -8,26 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C7B4C4-98D8-47F7-A249-23B637C1E674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F7939E-654A-4820-8C60-A7CBB58EF138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
   </bookViews>
   <sheets>
-    <sheet name="13SEP24_SWEEP_ON_FUEL" sheetId="7" r:id="rId1"/>
+    <sheet name="ET017_NIT013_AIR16_DIST" sheetId="10" r:id="rId1"/>
     <sheet name="23JUL24_SWEEP_ON_AIR" sheetId="8" r:id="rId2"/>
     <sheet name="20JUL24_SWEEP_ON_NITROGEN" sheetId="9" r:id="rId3"/>
+    <sheet name="13SEP24_SWEEP_ON_FUEL" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
   <si>
     <t>1:3</t>
   </si>
@@ -144,6 +156,60 @@
   </si>
   <si>
     <t>D:\Hamed\CND\PhD\Experiments\PFA-RH122\PFA results\SMPS\SMPS_laptop_datafiles_DEC24\Data\Raw</t>
+  </si>
+  <si>
+    <t>2024-07-26_143650_SMPS</t>
+  </si>
+  <si>
+    <t>1:2</t>
+  </si>
+  <si>
+    <t>2024-07-26_183046_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-30_160231_SMPS</t>
+  </si>
+  <si>
+    <t>2024-07-30_210108_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-19_183232_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-19_224826_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-20_125844_SMPS</t>
+  </si>
+  <si>
+    <t>1:4</t>
+  </si>
+  <si>
+    <t>2024-08-20_174346_SMPS</t>
+  </si>
+  <si>
+    <t>2:4</t>
+  </si>
+  <si>
+    <t>2024-08-20_183004_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-20_230112_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-21_194931_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-22_013117_SMPS</t>
+  </si>
+  <si>
+    <t>3:6</t>
+  </si>
+  <si>
+    <t>2024-08-28_191006_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-28_234919_SMPS</t>
   </si>
 </sst>
 </file>
@@ -153,7 +219,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +232,12 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -533,23 +605,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E154B3E6-2BDE-4817-B65C-F71F8F992F62}">
-  <dimension ref="A1:H48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AE73DF-AC79-457F-9CE4-E6FEFB9D1C73}">
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="1" max="1" width="68.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -566,161 +636,250 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4">
-        <v>20</v>
-      </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="4">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4">
-        <v>20</v>
-      </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="C28" s="5"/>
-      <c r="E28" s="4"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-    </row>
-    <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="4"/>
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="H48"/>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -729,7 +888,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,4 +1323,196 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E154B3E6-2BDE-4817-B65C-F71F8F992F62}">
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="4">
+        <v>20</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="C28" s="5"/>
+      <c r="E28" s="4"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="48" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="4"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Minor updates on input and visualization
</commit_message>
<xml_diff>
--- a/inputs/dma_params_new.xlsx
+++ b/inputs/dma_params_new.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F7939E-654A-4820-8C60-A7CBB58EF138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3466676D-5584-46E6-8A64-5C2B871C3E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
   </bookViews>
   <sheets>
-    <sheet name="ET017_NIT013_AIR16_DIST" sheetId="10" r:id="rId1"/>
-    <sheet name="23JUL24_SWEEP_ON_AIR" sheetId="8" r:id="rId2"/>
-    <sheet name="20JUL24_SWEEP_ON_NITROGEN" sheetId="9" r:id="rId3"/>
-    <sheet name="13SEP24_SWEEP_ON_FUEL" sheetId="7" r:id="rId4"/>
+    <sheet name="19AUG24_LOWAGGLOM_TANDEM" sheetId="11" r:id="rId1"/>
+    <sheet name="ET017_NIT013_AIR16_DIST" sheetId="10" r:id="rId2"/>
+    <sheet name="23JUL24_SWEEP_ON_AIR" sheetId="8" r:id="rId3"/>
+    <sheet name="20JUL24_SWEEP_ON_NITROGEN" sheetId="9" r:id="rId4"/>
+    <sheet name="13SEP24_SWEEP_ON_FUEL" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="67">
   <si>
     <t>1:3</t>
   </si>
@@ -210,6 +211,36 @@
   </si>
   <si>
     <t>2024-08-28_234919_SMPS</t>
+  </si>
+  <si>
+    <t>da (nm)</t>
+  </si>
+  <si>
+    <t>Qsh_AAC (lpm)</t>
+  </si>
+  <si>
+    <t>2024-08-19_190018_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-19_195449_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-19_204309_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-19_211132_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-19_212526_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-19_214004_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-19_215841_SMPS</t>
+  </si>
+  <si>
+    <t>2024-08-19_221858_SMPS</t>
   </si>
 </sst>
 </file>
@@ -605,11 +636,344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E29823-EAED-4A25-8B8F-59B6950B05BB}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="4">
+        <v>31.5</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2.84</v>
+      </c>
+      <c r="E2" s="5">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="4">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3.36</v>
+      </c>
+      <c r="E3" s="5">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="4">
+        <v>43.3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3.93</v>
+      </c>
+      <c r="E4" s="5">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="4">
+        <v>50.8</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4.62</v>
+      </c>
+      <c r="E5" s="5">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="4">
+        <v>59.5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="E6" s="5">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="4">
+        <v>69.7</v>
+      </c>
+      <c r="D7" s="4">
+        <v>6.33</v>
+      </c>
+      <c r="E7" s="5">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="4">
+        <v>81.7</v>
+      </c>
+      <c r="D8" s="4">
+        <v>7.41</v>
+      </c>
+      <c r="E8" s="5">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="4">
+        <v>95.8</v>
+      </c>
+      <c r="D9" s="4">
+        <v>8.67</v>
+      </c>
+      <c r="E9" s="5">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="4">
+        <v>112.3</v>
+      </c>
+      <c r="D10" s="4">
+        <v>10.09</v>
+      </c>
+      <c r="E10" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="4">
+        <v>131.6</v>
+      </c>
+      <c r="D11" s="4">
+        <v>11.25</v>
+      </c>
+      <c r="E11" s="5">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="4">
+        <v>154.30000000000001</v>
+      </c>
+      <c r="D12" s="4">
+        <v>12.53</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="4">
+        <v>180.8</v>
+      </c>
+      <c r="D13" s="4">
+        <v>13.86</v>
+      </c>
+      <c r="E13" s="5">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="4">
+        <v>211.9</v>
+      </c>
+      <c r="D14" s="4">
+        <v>15</v>
+      </c>
+      <c r="E14" s="5">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="5"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="5"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="5"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AE73DF-AC79-457F-9CE4-E6FEFB9D1C73}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,9 +1108,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
@@ -883,7 +1245,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E1FF8C-F2C6-4468-9BAB-5FF356FF2B49}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -1162,7 +1524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A154C9C-AB65-4231-8298-10E3CEF878B7}">
   <dimension ref="A1:H47"/>
   <sheetViews>
@@ -1325,7 +1687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E154B3E6-2BDE-4817-B65C-F71F8F992F62}">
   <dimension ref="A1:H48"/>
   <sheetViews>

</xml_diff>

<commit_message>
little updates on inputs and visuals
</commit_message>
<xml_diff>
--- a/inputs/dma_params_new.xlsx
+++ b/inputs/dma_params_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\hmdni\OneDrive\Documents\GitHub\odias\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D97F0C-E01F-4EDB-9891-FACD7AB487FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB370A68-9D8B-4B17-9DB8-9296ADDE2040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
+    <workbookView xWindow="5295" yWindow="2940" windowWidth="15060" windowHeight="11295" firstSheet="3" activeTab="3" xr2:uid="{BF76CB6B-6024-45E4-967E-95DB60FBF193}"/>
   </bookViews>
   <sheets>
     <sheet name="30JUL24_HIGHAGGLOM_TANDEM" sheetId="16" r:id="rId1"/>
@@ -849,7 +849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8233F0CA-20B3-4732-AA6F-4B7FCD80809C}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2188,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F64623-3178-4362-8C41-1BB89F188493}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2283,7 +2283,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="G4" s="4">
         <v>8</v>
@@ -2304,7 +2304,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G5" s="4">
         <v>8</v>
@@ -2325,7 +2325,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
         <v>8</v>
@@ -2430,7 +2430,7 @@
         <v>2.5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="G11" s="4">
         <v>8</v>
@@ -2450,7 +2450,7 @@
         <v>2.5</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="G12" s="4">
         <v>8</v>
@@ -2470,7 +2470,7 @@
         <v>2.5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="G13" s="4">
         <v>8</v>
@@ -2490,7 +2490,7 @@
         <v>2.5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G14" s="4">
         <v>8</v>

</xml_diff>